<commit_message>
Only testing for Bayes left
</commit_message>
<xml_diff>
--- a/DataClassification.xlsx
+++ b/DataClassification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Github\IS-Lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FACC7F6-E49C-4127-A0B3-34C36DF9565F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62B871A-BCC4-4F6B-A83A-9DD24A06049C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="64">
   <si>
     <t>T</t>
   </si>
@@ -109,6 +109,114 @@
   </si>
   <si>
     <t>x2</t>
+  </si>
+  <si>
+    <t>hsv_value_A4 hsv_value_A6 hsv_value_A7 hsv_value_A8 hsv_value_A9 hsv_value_P3 hsv_value_P4]</t>
+  </si>
+  <si>
+    <t>metric_A4 metric_A6 metric_A7 metric_A8 metric_A9 metric_P3 metric_P4]</t>
+  </si>
+  <si>
+    <t>hsv_value_A4 hsv</t>
+  </si>
+  <si>
+    <t>hsv_value_A1 hsv</t>
+  </si>
+  <si>
+    <t>hsv_value_A2 hsv</t>
+  </si>
+  <si>
+    <t>hsv_value_A3 hsv</t>
+  </si>
+  <si>
+    <t>hsv_value_A6 hsv</t>
+  </si>
+  <si>
+    <t>hsv_value_A7 hsv</t>
+  </si>
+  <si>
+    <t>hsv_value_A8 hsv</t>
+  </si>
+  <si>
+    <t>hsv_value_A9 hsv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metric_A4 </t>
+  </si>
+  <si>
+    <t>metric_A1</t>
+  </si>
+  <si>
+    <t>metric_A2</t>
+  </si>
+  <si>
+    <t>metric_A3</t>
+  </si>
+  <si>
+    <t>metric_A6</t>
+  </si>
+  <si>
+    <t>metric_A7</t>
+  </si>
+  <si>
+    <t>metric_A8</t>
+  </si>
+  <si>
+    <t>metric_A9</t>
+  </si>
+  <si>
+    <t>metric_P1</t>
+  </si>
+  <si>
+    <t>metric_P2</t>
+  </si>
+  <si>
+    <t>metric_P3</t>
+  </si>
+  <si>
+    <t>metric_P4</t>
+  </si>
+  <si>
+    <t>hsv_value_P1 hsv</t>
+  </si>
+  <si>
+    <t>hsv_value_P2 hsv</t>
+  </si>
+  <si>
+    <t>hsv_value_P3 hsv</t>
+  </si>
+  <si>
+    <t>hsv_value_P4 hsv</t>
+  </si>
+  <si>
+    <t>hsv_value_A5 hsv</t>
+  </si>
+  <si>
+    <t>metric_A5</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>DarkRed</t>
+  </si>
+  <si>
+    <t>YellowRed</t>
+  </si>
+  <si>
+    <t>LightGreen</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>LightBrown</t>
+  </si>
+  <si>
+    <t>Oval</t>
+  </si>
+  <si>
+    <t>SmallPearShape</t>
   </si>
 </sst>
 </file>
@@ -124,18 +232,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -150,10 +252,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,164 +535,165 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K52" sqref="K52"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="2" max="3" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.21834718250327201</v>
       </c>
       <c r="B2">
         <v>0.81883722366689804</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.14114915652447901</v>
       </c>
       <c r="B3">
         <v>0.83535287874573905</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.37021584902077798</v>
       </c>
       <c r="B4">
         <v>0.81110058002763896</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.14912715617648301</v>
       </c>
       <c r="B5">
         <v>0.771042136373982</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.184738799287993</v>
       </c>
       <c r="B6">
         <v>0.62789682435281402</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.21834718250327201</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>0.81883722366689804</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.14114915652447901</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>0.83535287874573905</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.37021584902077798</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>0.81110058002763896</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0.14912715617648301</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>0.771042136373982</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0.184738799287993</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>0.62789682435281402</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>9</v>
       </c>
     </row>
@@ -650,70 +752,262 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>26</v>
       </c>
       <c r="B49" t="s">
         <v>27</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>24</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" t="s">
         <v>11</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="D50" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>5</v>
       </c>
       <c r="B51" t="s">
         <v>12</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>25</v>
       </c>
       <c r="B52" t="s">
         <v>12</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>5</v>
       </c>
       <c r="B53" t="s">
         <v>9</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>7</v>
       </c>
       <c r="B54" t="s">
         <v>9</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>31</v>
+      </c>
+      <c r="B67" t="s">
+        <v>58</v>
+      </c>
+      <c r="D67" t="s">
+        <v>39</v>
+      </c>
+      <c r="E67" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>32</v>
+      </c>
+      <c r="B68" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68" t="s">
+        <v>40</v>
+      </c>
+      <c r="E68" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>33</v>
+      </c>
+      <c r="B69" t="s">
+        <v>58</v>
+      </c>
+      <c r="D69" t="s">
+        <v>41</v>
+      </c>
+      <c r="E69" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>30</v>
+      </c>
+      <c r="B70" t="s">
+        <v>58</v>
+      </c>
+      <c r="D70" t="s">
+        <v>38</v>
+      </c>
+      <c r="E70" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>54</v>
+      </c>
+      <c r="B71" t="s">
+        <v>56</v>
+      </c>
+      <c r="D71" t="s">
+        <v>55</v>
+      </c>
+      <c r="E71" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>34</v>
+      </c>
+      <c r="B72" t="s">
+        <v>56</v>
+      </c>
+      <c r="D72" t="s">
+        <v>42</v>
+      </c>
+      <c r="E72" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>35</v>
+      </c>
+      <c r="B73" t="s">
+        <v>57</v>
+      </c>
+      <c r="D73" t="s">
+        <v>43</v>
+      </c>
+      <c r="E73" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>36</v>
+      </c>
+      <c r="B74" t="s">
+        <v>58</v>
+      </c>
+      <c r="D74" t="s">
+        <v>44</v>
+      </c>
+      <c r="E74" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>37</v>
+      </c>
+      <c r="B75" t="s">
+        <v>56</v>
+      </c>
+      <c r="D75" t="s">
+        <v>45</v>
+      </c>
+      <c r="E75" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>50</v>
+      </c>
+      <c r="B76" t="s">
+        <v>59</v>
+      </c>
+      <c r="D76" t="s">
+        <v>46</v>
+      </c>
+      <c r="E76" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>51</v>
+      </c>
+      <c r="B77" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77" t="s">
+        <v>47</v>
+      </c>
+      <c r="E77" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>52</v>
+      </c>
+      <c r="B78" t="s">
+        <v>60</v>
+      </c>
+      <c r="D78" t="s">
+        <v>48</v>
+      </c>
+      <c r="E78" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>53</v>
+      </c>
+      <c r="B79" t="s">
+        <v>61</v>
+      </c>
+      <c r="D79" t="s">
+        <v>49</v>
+      </c>
+      <c r="E79" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>